<commit_message>
added dynamic visual questions
</commit_message>
<xml_diff>
--- a/uploads/input.xlsx
+++ b/uploads/input.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishay\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6511D8-3A7B-48CC-AC82-D0C9D67A03DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
   <si>
     <t>שאלה</t>
   </si>
@@ -129,12 +135,45 @@
   </si>
   <si>
     <t>לא</t>
+  </si>
+  <si>
+    <t>סליידר</t>
+  </si>
+  <si>
+    <t>check box</t>
+  </si>
+  <si>
+    <t>מזון מהצומח כולל: דגנים, קטניות, פירות וירקות.  
+מזון מהחי כולל: בשר, עוף, דגים, ביצים, מוצרי חלב.  
+לפי ההגדרה הזאת, איזה אחוז מהתזונה שלך מבוסס על מזונות מהצומח? החליקי למענה</t>
+  </si>
+  <si>
+    <t>סביבה</t>
+  </si>
+  <si>
+    <t>בקניית מזון אורגני, אנא צייני איפה את רוכשת את המוצרים:
+(אפשר לסמן יותר מתשובה אחת)</t>
+  </si>
+  <si>
+    <t>ישירות מהחקלאי</t>
+  </si>
+  <si>
+    <t>בחנות קטנה בעיר</t>
+  </si>
+  <si>
+    <t>בעסק חברתי</t>
+  </si>
+  <si>
+    <t>ברשת שיווק</t>
+  </si>
+  <si>
+    <t>גידול עצמי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -142,7 +181,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -184,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
@@ -192,6 +231,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -208,10 +250,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,28 +573,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.75" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="35.44140625" customWidth="1"/>
-    <col min="18" max="18" width="14.77734375" customWidth="1"/>
+    <col min="17" max="17" width="35.5" customWidth="1"/>
+    <col min="18" max="18" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +650,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -650,11 +688,11 @@
         <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N2">
         <f>IF(M2=C2,0,IF(M2=D2,1,IF(M2=E2,2,IF(M2=F2,3,99))))</f>
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
@@ -669,7 +707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -707,11 +745,11 @@
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <f>IF(M3=C3,3,IF(M3=D3,2,IF(M3=E3,1,IF(M3=F3,0,99))))</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -726,7 +764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -764,11 +802,11 @@
         <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N4">
         <f>IF(M4=C4,0,IF(M4=D4,1,IF(M4=E4,2,IF(M4=F4,3,99))))</f>
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="O4" t="s">
         <v>25</v>
@@ -783,7 +821,122 @@
         <v>24</v>
       </c>
     </row>
+    <row r="5" spans="1:18" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="str">
+        <f>M5</f>
+        <v>NA</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{4FFB17DC-E62A-4686-860A-306ACF5888CC}">
+      <formula1>"אמריקאית,סליידר,check box"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add functions that read ans write to excel file
</commit_message>
<xml_diff>
--- a/uploads/input.xlsx
+++ b/uploads/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishay\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6511D8-3A7B-48CC-AC82-D0C9D67A03DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F57CAE-7A02-4C45-90DB-EC212E94EA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
+    <sheet name="A" sheetId="1" r:id="rId1"/>
+    <sheet name="B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="45">
   <si>
     <t>שאלה</t>
   </si>
@@ -576,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -691,7 +692,7 @@
         <v>24</v>
       </c>
       <c r="N2">
-        <f>IF(M2=C2,0,IF(M2=D2,1,IF(M2=E2,2,IF(M2=F2,3,99))))</f>
+        <f>IF(TRIM(B!A2)=TRIM(C2),0,IF(TRIM(B!A2)=TRIM(D2),1,IF(TRIM(B!A2)=TRIM(E2),2,IF(TRIM(B!A2)=TRIM(F2),3,99))))</f>
         <v>99</v>
       </c>
       <c r="O2" t="s">
@@ -707,7 +708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -748,7 +749,7 @@
         <v>24</v>
       </c>
       <c r="N3">
-        <f>IF(M3=C3,3,IF(M3=D3,2,IF(M3=E3,1,IF(M3=F3,0,99))))</f>
+        <f>IF(TRIM(B!A3)=TRIM(C3),0,IF(TRIM(B!A3)=TRIM(D3),1,IF(TRIM(B!A3)=TRIM(E3),2,IF(TRIM(B!A3)=TRIM(F3),3,99))))</f>
         <v>99</v>
       </c>
       <c r="O3" t="s">
@@ -764,7 +765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -805,7 +806,7 @@
         <v>24</v>
       </c>
       <c r="N4">
-        <f>IF(M4=C4,0,IF(M4=D4,1,IF(M4=E4,2,IF(M4=F4,3,99))))</f>
+        <f>IF(TRIM(B!A4)=TRIM(C4),0,IF(TRIM(B!A4)=TRIM(D4),1,IF(TRIM(B!A4)=TRIM(E4),2,IF(TRIM(B!A4)=TRIM(F4),3,99))))</f>
         <v>99</v>
       </c>
       <c r="O4" t="s">
@@ -862,7 +863,7 @@
         <v>24</v>
       </c>
       <c r="N5" t="str">
-        <f>M5</f>
+        <f>B!A5</f>
         <v>NA</v>
       </c>
       <c r="O5" t="s">
@@ -918,8 +919,9 @@
       <c r="M6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="s">
-        <v>24</v>
+      <c r="N6" t="str">
+        <f>N5</f>
+        <v>NA</v>
       </c>
       <c r="O6" t="s">
         <v>36</v>
@@ -940,4 +942,978 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C04606-201A-48A4-BD8C-C067EA1045EE}">
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added writing of checkbox answers to excel
</commit_message>
<xml_diff>
--- a/uploads/input.xlsx
+++ b/uploads/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\share_projects\final_project\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA5333B-1D31-4615-8781-1CA15DD9E252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE4F2FB-DF07-4065-9477-859C501FCA87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="60">
   <si>
     <t>תשובה1</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>תשובה10</t>
-  </si>
-  <si>
-    <t>תשובת משתמש</t>
   </si>
   <si>
     <t>חישוב סופי</t>
@@ -184,6 +181,39 @@
   <si>
     <t>בקניית מזון אורגני, אנא ציין איפה אתה רוכש את המוצרים:
 (אפשר לסמן יותר מתשובה אחת)</t>
+  </si>
+  <si>
+    <t>תשובת משתמש1</t>
+  </si>
+  <si>
+    <t>תשובת משתמש2</t>
+  </si>
+  <si>
+    <t>תשובת משתמש3</t>
+  </si>
+  <si>
+    <t>תשובת משתמש4</t>
+  </si>
+  <si>
+    <t>תשובת משתמש5</t>
+  </si>
+  <si>
+    <t>תשובת משתמש6</t>
+  </si>
+  <si>
+    <t>תשובת משתמש7</t>
+  </si>
+  <si>
+    <t>תשובת משתמש8</t>
+  </si>
+  <si>
+    <t>תשובת משתמש9</t>
+  </si>
+  <si>
+    <t>תשובת משתמש10</t>
+  </si>
+  <si>
+    <t>NON</t>
   </si>
 </sst>
 </file>
@@ -239,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
@@ -251,6 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N4" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -603,22 +634,23 @@
     <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.75" customWidth="1"/>
-    <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="18" max="18" width="35.5" customWidth="1"/>
-    <col min="19" max="19" width="14.75" customWidth="1"/>
+    <col min="14" max="14" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="35.5" customWidth="1"/>
+    <col min="18" max="18" width="14.75" customWidth="1"/>
+    <col min="19" max="19" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -654,325 +686,1014 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="Q1" t="s">
         <v>31</v>
       </c>
       <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2">
+        <f>N3</f>
+        <v>99</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3">
+        <f>IF(TRIM(S3)=TRIM(D3),0,IF(TRIM(S3)=TRIM(E3),1,IF(TRIM(S3)=TRIM(F3),2,IF(TRIM(S3)=TRIM(G3),3,99))))</f>
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="S3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4">
+        <f>IF(TRIM(S4)=TRIM(D4),0,IF(TRIM(S4)=TRIM(E4),1,IF(TRIM(S4)=TRIM(F4),2,IF(TRIM(S4)=TRIM(G4),3,99))))</f>
+        <v>99</v>
+      </c>
+      <c r="O4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2">
-        <f>IF(TRIM(A2)=TRIM(D2),0,IF(TRIM(A2)=TRIM(E2),1,IF(TRIM(A2)=TRIM(F2),2,IF(TRIM(A2)=TRIM(G2),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="str">
+        <f>S5</f>
+        <v>NON</v>
+      </c>
+      <c r="O5" t="s">
         <v>33</v>
       </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3">
-        <f>IF(TRIM(A3)=TRIM(D3),0,IF(TRIM(A3)=TRIM(E3),1,IF(TRIM(A3)=TRIM(F3),2,IF(TRIM(A3)=TRIM(G3),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4">
-        <f>IF(TRIM(A4)=TRIM(D4),0,IF(TRIM(A4)=TRIM(E4),1,IF(TRIM(A4)=TRIM(F4),2,IF(TRIM(A4)=TRIM(G4),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="126" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" t="str">
-        <f>A5</f>
-        <v>מזון מהצומח כולל: דגנים, קטניות, פירות וירקות.  
-מזון מהחי כולל: בשר, עוף, דגים, ביצים, מוצרי חלב.  
-לפי ההגדרה הזאת, איזה אחוז מהתזונה שלך מבוסס על מזונות מהצומח? החליקי למענה</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="e">
+        <f>(IF(S6=D6,1,0) + IF(T6=E6,2,0) +  IF(U6=F6,3,0) +  IF(V6=G6,4,0) +  IF(W6=H6,5,0) +  IF(X6=I6,5,0) +  IF(Y6=J6,5,0) +  IF(Z6=K6,5,0) +  IF(AA6=L6,5,0) +  IF(AB6=M6,5,0))/ (IF(S6=D6,1,0) + IF(T6=E6,1,0) +  IF(U6=F6,1,0) +  IF(V6=G6,1,0) +  IF(W6=H6,1,0) +  IF(X6=I6,1,0) +  IF(Y6=J6,1,0) +  IF(Z6=K6,1,0) +  IF(AA6=L6,1,0) +  IF(AB6=M6,1,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" t="str">
-        <f>O5</f>
-        <v>מזון מהצומח כולל: דגנים, קטניות, פירות וירקות.  
-מזון מהחי כולל: בשר, עוף, דגים, ביצים, מוצרי חלב.  
-לפי ההגדרה הזאת, איזה אחוז מהתזונה שלך מבוסס על מזונות מהצומח? החליקי למענה</v>
-      </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="R6" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+    </row>
+    <row r="18" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+    </row>
+    <row r="19" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+    </row>
+    <row r="20" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+    </row>
+    <row r="21" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+    </row>
+    <row r="22" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+    </row>
+    <row r="23" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+    </row>
+    <row r="24" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+    </row>
+    <row r="25" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+    </row>
+    <row r="26" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+    </row>
+    <row r="27" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+    </row>
+    <row r="28" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+    </row>
+    <row r="29" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+    </row>
+    <row r="30" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+    </row>
+    <row r="31" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
+    </row>
+    <row r="32" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+    </row>
+    <row r="33" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+    </row>
+    <row r="34" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="5"/>
+    </row>
+    <row r="35" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+    </row>
+    <row r="36" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="5"/>
+    </row>
+    <row r="37" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="5"/>
+    </row>
+    <row r="38" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="5"/>
+    </row>
+    <row r="39" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5"/>
+    </row>
+    <row r="40" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="5"/>
+    </row>
+    <row r="41" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="5"/>
+    </row>
+    <row r="42" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="5"/>
+    </row>
+    <row r="43" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="5"/>
+    </row>
+    <row r="44" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="5"/>
+    </row>
+    <row r="45" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5"/>
+    </row>
+    <row r="46" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5"/>
+    </row>
+    <row r="47" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+    </row>
+    <row r="48" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+    </row>
+    <row r="49" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="5"/>
+    </row>
+    <row r="50" spans="19:28" x14ac:dyDescent="0.25">
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{4FFB17DC-E62A-4686-860A-306ACF5888CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{4FFB17DC-E62A-4686-860A-306ACF5888CC}">
       <formula1>"אמריקאית,סליידר,check box"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>